<commit_message>
Sync local changes before rebase
</commit_message>
<xml_diff>
--- a/new_test_data/new_data.xlsx
+++ b/new_test_data/new_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ppp\mlops_churn_prediction\new_test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D31B9CA6-5BBA-4AA4-8A7F-59E81E5A7B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2A6427-C216-4977-B434-494B205F098E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{35DDD86D-9455-41ED-AA9A-23247E548272}"/>
   </bookViews>
@@ -559,15 +559,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{990B83D0-42A7-4739-919F-2D7E26BE341F}">
-  <dimension ref="A1:AI6"/>
+  <dimension ref="A1:AI5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AG14" sqref="AG14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="32" max="32" width="11.109375" customWidth="1"/>
+    <col min="33" max="33" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
@@ -768,6 +770,21 @@
       <c r="AD2">
         <v>65.2</v>
       </c>
+      <c r="AE2">
+        <v>2315.6999999999998</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>100</v>
+      </c>
+      <c r="AH2">
+        <v>406.3</v>
+      </c>
+      <c r="AI2">
+        <v>2722</v>
+      </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -861,19 +878,19 @@
         <v>102.3</v>
       </c>
       <c r="AE3">
-        <v>2315.6999999999998</v>
+        <v>784.2</v>
       </c>
       <c r="AF3">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="AG3">
         <v>0</v>
       </c>
       <c r="AH3">
-        <v>406.3</v>
+        <v>318.8</v>
       </c>
       <c r="AI3">
-        <v>2722</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.3">
@@ -968,19 +985,19 @@
         <v>54.1</v>
       </c>
       <c r="AE4">
-        <v>784.2</v>
+        <v>162.30000000000001</v>
       </c>
       <c r="AF4">
         <v>0</v>
       </c>
       <c r="AG4">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AH4">
-        <v>318.8</v>
+        <v>29.3</v>
       </c>
       <c r="AI4">
-        <v>1103</v>
+        <v>191.6</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.3">
@@ -1075,35 +1092,18 @@
         <v>110.9</v>
       </c>
       <c r="AE5">
-        <v>162.30000000000001</v>
+        <v>2450.5</v>
       </c>
       <c r="AF5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AG5">
         <v>0</v>
       </c>
       <c r="AH5">
-        <v>29.3</v>
+        <v>596.20000000000005</v>
       </c>
       <c r="AI5">
-        <v>191.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="AE6">
-        <v>2450.5</v>
-      </c>
-      <c r="AF6">
-        <v>10</v>
-      </c>
-      <c r="AG6">
-        <v>0</v>
-      </c>
-      <c r="AH6">
-        <v>596.20000000000005</v>
-      </c>
-      <c r="AI6">
         <v>3056.7</v>
       </c>
     </row>

</xml_diff>